<commit_message>
Update pricing, fix bug
</commit_message>
<xml_diff>
--- a/Design/Pricing.xlsx
+++ b/Design/Pricing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bsd405-my.sharepoint.com/personal/s-vikramadityan_bsd405_org/Documents/Tektite/TektiteR/RoTo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="271" documentId="8_{355650BB-0AA2-E14E-AC49-163D93A781F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CA33768-D4D2-844D-B4EC-E93F41C7ACC7}"/>
+  <xr:revisionPtr revIDLastSave="301" documentId="8_{355650BB-0AA2-E14E-AC49-163D93A781F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5290CBA6-C15E-3148-8BD4-7571E90B6A65}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{3323777E-1DF2-4348-B326-362B318325C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{3323777E-1DF2-4348-B326-362B318325C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Item</t>
   </si>
@@ -92,9 +92,6 @@
     <t>https://www.aliexpress.us/item/3256802013721550.html</t>
   </si>
   <si>
-    <t>https://banebots.com/banebots-wheel-2-7-8-x-0-8-hub-mount-30a-green/</t>
-  </si>
-  <si>
     <t>https://www.aliexpress.us/item/2251832479258088.html</t>
   </si>
   <si>
@@ -165,6 +162,30 @@
   </si>
   <si>
     <t>Need 4/8, NOT INCLUDED WITH KIT</t>
+  </si>
+  <si>
+    <t>Come with the pulleys I ordered for EV</t>
+  </si>
+  <si>
+    <t>M4 Set Screws</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B01N76NKU6</t>
+  </si>
+  <si>
+    <t>M4 Nut</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0BLBLM2BQ/</t>
+  </si>
+  <si>
+    <t>https://banebots.com/t61p-241by/</t>
+  </si>
+  <si>
+    <t>Button caps</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.us/item/2251832666419248.html</t>
   </si>
 </sst>
 </file>
@@ -269,6 +290,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -588,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DC6279-EE2D-524A-AEA0-F780B55F0CE3}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,7 +654,7 @@
       </c>
       <c r="H1" s="6">
         <f>SUM(E:E)</f>
-        <v>78.984944300000009</v>
+        <v>79.234871299999995</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -676,26 +701,26 @@
         <v>10</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="C4" s="5">
-        <f>3.5*1.101</f>
-        <v>3.8534999999999999</v>
+        <f>3.3*1.101</f>
+        <v>3.6332999999999998</v>
       </c>
       <c r="D4" s="9">
         <v>2</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ref="E4:E16" si="0">C4*D4</f>
-        <v>7.7069999999999999</v>
+        <f t="shared" ref="E4:E19" si="0">C4*D4</f>
+        <v>7.2665999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5">
         <f>15.09*1.101</f>
@@ -712,10 +737,10 @@
     </row>
     <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="5">
         <f>2.29*1.101</f>
@@ -729,15 +754,15 @@
         <v>5.0425800000000001</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5">
         <f>0.72*1.101</f>
@@ -753,10 +778,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5">
         <f>0.93*1.101</f>
@@ -772,10 +797,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="C9" s="5">
         <f>1.95*1.101</f>
@@ -791,10 +816,10 @@
     </row>
     <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>30</v>
       </c>
       <c r="C10" s="5">
         <f>4.99*1.101</f>
@@ -809,12 +834,12 @@
         <v>0.2197596</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>7</v>
@@ -832,15 +857,15 @@
         <v>0.63417599999999996</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="C12" s="5">
         <f>6.19*1.101</f>
@@ -855,15 +880,15 @@
         <v>1.590211</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="C13" s="5">
         <f>1.101*5.99</f>
@@ -878,15 +903,15 @@
         <v>0.19784969999999999</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="C14" s="5">
         <f>12.34*1.101</f>
@@ -900,46 +925,109 @@
         <v>0</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="5">
+        <f>7.09*1.101</f>
+        <v>7.8060899999999993</v>
+      </c>
+      <c r="D15" s="9">
+        <f>2/50</f>
+        <v>0.04</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>0.31224359999999995</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="5">
+        <f>5.99*1.101</f>
+        <v>6.5949900000000001</v>
+      </c>
+      <c r="D16" s="9">
+        <f>4/100</f>
+        <v>0.04</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.26379960000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="5">
+        <f>(0.94*2 + 3.31)*1.101</f>
+        <v>5.7141899999999994</v>
+      </c>
+      <c r="D17" s="9">
+        <f>1/50</f>
+        <v>0.02</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.11428379999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C18" s="5">
         <f>206.29-6</f>
         <v>200.29</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D18" s="9">
         <f>1/10</f>
         <v>0.1</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E18" s="5">
         <f t="shared" si="0"/>
         <v>20.029</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F18" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C19" s="5">
         <v>0</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D19" s="9">
         <v>1</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E19" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -947,7 +1035,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{D3B435A3-CA86-464A-A059-1F86BC2B6302}"/>
-    <hyperlink ref="B15" r:id="rId2" xr:uid="{B251EDFF-D916-5B47-9C82-AE2C63A918C4}"/>
+    <hyperlink ref="B18" r:id="rId2" xr:uid="{B251EDFF-D916-5B47-9C82-AE2C63A918C4}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{32EA09CA-016F-3D43-A8B7-94E4B11169EF}"/>
     <hyperlink ref="B2" r:id="rId4" xr:uid="{1127F7E8-945F-6540-8786-B8DD605BE466}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{E4AB4FCE-6424-BB48-BA05-6A379246494F}"/>
@@ -960,6 +1048,9 @@
     <hyperlink ref="B12" r:id="rId12" xr:uid="{802A29AB-5C3C-6442-98FE-17563A9601E1}"/>
     <hyperlink ref="B13" r:id="rId13" xr:uid="{9CDB432A-FF9A-E54B-82CE-78F7498E859B}"/>
     <hyperlink ref="B14" r:id="rId14" xr:uid="{16F69667-7B42-C14F-AE6B-337DBF9B7C60}"/>
+    <hyperlink ref="B15" r:id="rId15" xr:uid="{001FD839-99FA-3444-9DC6-F8D642CCDCCF}"/>
+    <hyperlink ref="B16" r:id="rId16" xr:uid="{D80B5B35-7DDE-FF4E-AA46-5793E4A4E067}"/>
+    <hyperlink ref="B17" r:id="rId17" xr:uid="{9C7B787C-AFDB-D341-934E-E23CEA48C744}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>